<commit_message>
Change Logic -> add 2 function
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -432,6 +432,11 @@
           <t>Pipe , ASME B36.10 , Beveled End , ASTM A53-B , Electric Resistance Welded (Ej =0.85), SCH/THK S-STD</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Pipe</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>